<commit_message>
Ajustado projeto para atender regras da PEP8
</commit_message>
<xml_diff>
--- a/data/gold/gold_sla_distribution.xlsx
+++ b/data/gold/gold_sla_distribution.xlsx
@@ -439,29 +439,25 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>Atendido</t>
-        </is>
+      <c r="A2" t="b">
+        <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>667</v>
+        <v>137</v>
       </c>
       <c r="C2" t="n">
-        <v>82.95999999999999</v>
+        <v>17.04</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>Violado</t>
-        </is>
+      <c r="A3" t="b">
+        <v>1</v>
       </c>
       <c r="B3" t="n">
-        <v>137</v>
+        <v>667</v>
       </c>
       <c r="C3" t="n">
-        <v>17.04</v>
+        <v>82.95999999999999</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Terceiro commit: Ingestão do Blob
</commit_message>
<xml_diff>
--- a/data/gold/gold_sla_distribution.xlsx
+++ b/data/gold/gold_sla_distribution.xlsx
@@ -439,25 +439,29 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="b">
-        <v>0</v>
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>atendido</t>
+        </is>
       </c>
       <c r="B2" t="n">
-        <v>137</v>
+        <v>667</v>
       </c>
       <c r="C2" t="n">
-        <v>17.04</v>
+        <v>82.95999999999999</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="b">
-        <v>1</v>
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>violado</t>
+        </is>
       </c>
       <c r="B3" t="n">
-        <v>667</v>
+        <v>137</v>
       </c>
       <c r="C3" t="n">
-        <v>82.95999999999999</v>
+        <v>17.04</v>
       </c>
     </row>
   </sheetData>

</xml_diff>